<commit_message>
Actualiza archivos de descarga de autogestion xlsx
</commit_message>
<xml_diff>
--- a/build/assets/statics/bdb/ACTUALIZACION.xlsx
+++ b/build/assets/statics/bdb/ACTUALIZACION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\squijano\Desktop\BANCO DE BOGOTA\ARCHIVOS AUTOGESTION CEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26F02B-C1A1-4290-8CC1-EEEEDE698806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70178A5-3195-4835-AFE3-A60E7282DB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="473" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1083,7 +1083,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5785,7 +5785,7 @@
       <c r="G507" s="12"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mRux5ni995BQGxNPKm7uwT68M9NPmIVUBzXoBdFtixWf9boKst6cjQlzzSxZxjjkYHpijrm1mFZlbT6Y7Ipq4g==" saltValue="O0oRHBI8Lu7yq9pD4gm8hA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0IkMoBCleR0qdRewUD2v6NNurMTCXkvqbeSlNjb1++QUoSsZAyUFd/DomzoOCl+dD9jifhojpxlYkkQIrXioDw==" saltValue="nC1KYbgZ76X+EYoIvPAKCg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="A8:N9 H7:N7 A10:G507" name="Rango1_1"/>
   </protectedRanges>

</xml_diff>

<commit_message>
Actualiza archivo de ACTUALIZACION
</commit_message>
<xml_diff>
--- a/build/assets/statics/bdb/ACTUALIZACION.xlsx
+++ b/build/assets/statics/bdb/ACTUALIZACION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\squijano\Desktop\BANCO DE BOGOTA\ARCHIVOS AUTOGESTION CEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70178A5-3195-4835-AFE3-A60E7282DB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EBE988-D3D2-4B84-9648-589FE8FAB1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="473" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1083,7 +1083,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5785,7 +5785,7 @@
       <c r="G507" s="12"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="0IkMoBCleR0qdRewUD2v6NNurMTCXkvqbeSlNjb1++QUoSsZAyUFd/DomzoOCl+dD9jifhojpxlYkkQIrXioDw==" saltValue="nC1KYbgZ76X+EYoIvPAKCg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+nCPhVXYu2Q/wrNKu9jeklRFuFEFntsib0gKA4NxCKjErAwCeGQesd68PsLpSAw1MzID61034WAwhb24CSaTEg==" saltValue="rE5wxvK3Qns4YMAk8fB3kw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="A8:N9 H7:N7 A10:G507" name="Rango1_1"/>
   </protectedRanges>

</xml_diff>